<commit_message>
[project] More ACS amendments
 - Data documentation
 - example analysis
 - extract routine
 - source table
</commit_message>
<xml_diff>
--- a/data-raw/acs_lus.xlsx
+++ b/data-raw/acs_lus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53DFBD88-D89D-4CA4-B2A8-F9B9633E4407}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1349A4CB-DCD0-46D8-9C31-85CDD6BFEACA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="12570" windowHeight="7770" tabRatio="345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,12 +34,12 @@
     <definedName name="HTML_PathFile" hidden="1">"G:\ACTIVITY\HELP\DTPANIC\2001-02\MyHTML.htm"</definedName>
     <definedName name="HTML_Title" hidden="1">"Section 1"</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="139">
   <si>
     <t>Prepared by:</t>
   </si>
@@ -392,15 +392,9 @@
     <t>K[0-4]|K5[025-7]|K6[016-9]|K7[134]</t>
   </si>
   <si>
-    <t>sec_diag_regex</t>
-  </si>
-  <si>
     <t>prim_diag_regexp</t>
   </si>
   <si>
-    <t>proc_regex</t>
-  </si>
-  <si>
     <t>I50|I110|J81X|I130</t>
   </si>
   <si>
@@ -450,6 +444,18 @@
   </si>
   <si>
     <t>-K0-K4;-K50;-K52;-K55-K57;-K60-K61;-K67-K69;-K71;-K73-K74</t>
+  </si>
+  <si>
+    <t>sec_diag_exclude_regexp</t>
+  </si>
+  <si>
+    <t>proc_exclude_regexp</t>
+  </si>
+  <si>
+    <t>sec_diag_include_regexp</t>
+  </si>
+  <si>
+    <t>D57</t>
   </si>
 </sst>
 </file>
@@ -1471,14 +1477,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6428CD34-B99A-449C-BD75-92CB38E0302C}" name="Table225" displayName="Table225" ref="A1:J14" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:J14" xr:uid="{34C5B988-CB0B-48F9-8C55-CD3937E4AD79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6428CD34-B99A-449C-BD75-92CB38E0302C}" name="Table225" displayName="Table225" ref="A1:K14" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:K14" xr:uid="{34C5B988-CB0B-48F9-8C55-CD3937E4AD79}"/>
   <sortState ref="A2:G14">
     <sortCondition ref="A2:A34"/>
     <sortCondition ref="B2:B34"/>
     <sortCondition ref="E2:E34"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="4" xr3:uid="{24E9D885-27DA-485D-8ED9-0816ADED6CA2}" name="cat1"/>
     <tableColumn id="6" xr3:uid="{13906DF1-45F9-4BB4-8432-0BDA25CBF305}" name="cat2"/>
     <tableColumn id="1" xr3:uid="{9E861F73-7DDD-43B0-A504-64B3944D7CC4}" name="Condition description"/>
@@ -1487,8 +1493,9 @@
     <tableColumn id="5" xr3:uid="{1333528A-B35E-42D7-8D0D-BDA8148950B2}" name="secondary diagnoses" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{552BB330-A267-471F-AA74-BB143F22FC48}" name="procedures"/>
     <tableColumn id="10" xr3:uid="{37FDC531-A372-42C5-9DCA-F71DE66EAF52}" name="prim_diag_regexp"/>
-    <tableColumn id="8" xr3:uid="{8A4925F4-E557-4EB8-BC6C-9D14C98E5FD9}" name="proc_regex"/>
-    <tableColumn id="9" xr3:uid="{152684CE-BB8F-4D6A-B72F-F7F80E6C2980}" name="sec_diag_regex"/>
+    <tableColumn id="9" xr3:uid="{152684CE-BB8F-4D6A-B72F-F7F80E6C2980}" name="sec_diag_include_regexp"/>
+    <tableColumn id="11" xr3:uid="{6699B0AE-5515-43B6-A543-9132AD06FA71}" name="sec_diag_exclude_regexp"/>
+    <tableColumn id="8" xr3:uid="{8A4925F4-E557-4EB8-BC6C-9D14C98E5FD9}" name="proc_exclude_regexp"/>
   </tableColumns>
   <tableStyleInfo name="NCC White Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2468,10 +2475,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645F42B4-D193-4C4D-8A1D-36E8399E4942}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2483,10 +2490,11 @@
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -2509,16 +2517,19 @@
         <v>104</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -2535,12 +2546,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -2554,16 +2565,16 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -2577,16 +2588,16 @@
       <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2595,16 +2606,16 @@
         <v>105</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" t="s">
+        <v>118</v>
+      </c>
+      <c r="K5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -2618,21 +2629,21 @@
         <v>111</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
-      </c>
-      <c r="I6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -2641,15 +2652,15 @@
         <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -2661,13 +2672,14 @@
         <v>101</v>
       </c>
       <c r="H8" t="s">
-        <v>124</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="I8" s="10"/>
       <c r="J8" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2681,10 +2693,10 @@
         <v>109</v>
       </c>
       <c r="H9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2698,10 +2710,10 @@
         <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2715,10 +2727,10 @@
         <v>106</v>
       </c>
       <c r="H11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -2732,10 +2744,10 @@
         <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -2749,16 +2761,16 @@
         <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H13" t="s">
         <v>41</v>
       </c>
-      <c r="J13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2772,7 +2784,7 @@
         <v>108</v>
       </c>
       <c r="H14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[project] Adapt ac for no version in conditions.  Expand conditions.
</commit_message>
<xml_diff>
--- a/data-raw/acs_lus.xlsx
+++ b/data-raw/acs_lus.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1349A4CB-DCD0-46D8-9C31-85CDD6BFEACA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66279789-0A59-4E66-A20F-90D0D8BB51AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="12570" windowHeight="7770" tabRatio="345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="12570" windowHeight="7770" tabRatio="421" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="ACS meta" sheetId="17" r:id="rId2"/>
-    <sheet name="ACS detail" sheetId="18" r:id="rId3"/>
+    <sheet name="ccg_ois_26_detail" sheetId="18" r:id="rId3"/>
     <sheet name="ccg_ois_26" sheetId="19" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -34,12 +34,12 @@
     <definedName name="HTML_PathFile" hidden="1">"G:\ACTIVITY\HELP\DTPANIC\2001-02\MyHTML.htm"</definedName>
     <definedName name="HTML_Title" hidden="1">"Section 1"</definedName>
   </definedNames>
-  <calcPr calcId="179017" calcMode="manual"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="134">
   <si>
     <t>Prepared by:</t>
   </si>
@@ -71,15 +71,6 @@
     <t>Condition description</t>
   </si>
   <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>COPD</t>
-  </si>
-  <si>
-    <t>All ages</t>
-  </si>
-  <si>
     <t>I20</t>
   </si>
   <si>
@@ -296,15 +287,9 @@
     <t>cat2</t>
   </si>
   <si>
-    <t>Hepatitis B</t>
-  </si>
-  <si>
     <t>Diabetes</t>
   </si>
   <si>
-    <t>CHD</t>
-  </si>
-  <si>
     <t>Hypertension</t>
   </si>
   <si>
@@ -314,9 +299,6 @@
     <t>Dementia</t>
   </si>
   <si>
-    <t>Anaemia</t>
-  </si>
-  <si>
     <t>primary diagnosis</t>
   </si>
   <si>
@@ -377,12 +359,6 @@
     <t>I10X;I11.9</t>
   </si>
   <si>
-    <t>COPD (secondary)</t>
-  </si>
-  <si>
-    <t>COPD (primary)</t>
-  </si>
-  <si>
     <t>D51-D52;D50.1;D50.8;D50.9</t>
   </si>
   <si>
@@ -456,6 +432,15 @@
   </si>
   <si>
     <t>D57</t>
+  </si>
+  <si>
+    <t>primary diagnosis detail</t>
+  </si>
+  <si>
+    <t>COPD (acute)</t>
+  </si>
+  <si>
+    <t>COPD (chronic)</t>
   </si>
 </sst>
 </file>
@@ -465,7 +450,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -530,6 +515,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -579,7 +570,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -608,6 +599,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink 2" xfId="13" xr:uid="{07EDB42A-E988-4E59-B5DC-C1AF434549F1}"/>
@@ -625,7 +621,29 @@
     <cellStyle name="Normal 5 2" xfId="6" xr:uid="{E757CAE4-A39C-4AE3-95B2-8A65678088A1}"/>
     <cellStyle name="Normal 6 2 2" xfId="4" xr:uid="{B0B1FA75-ACA4-424E-8D9B-3DC7352572AB}"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.499984740745262"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -998,42 +1016,42 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="NCC White Table" defaultPivotStyle="NCC White Pivot">
     <tableStyle name="NCC White Pivot" table="0" count="11" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="36"/>
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="totalRow" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="31"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="30"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="29"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="28"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="27"/>
-      <tableStyleElement type="pageFieldValues" dxfId="26"/>
+      <tableStyleElement type="wholeTable" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="37"/>
+      <tableStyleElement type="totalRow" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="34"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="33"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="32"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="31"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="30"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="29"/>
+      <tableStyleElement type="pageFieldValues" dxfId="28"/>
     </tableStyle>
     <tableStyle name="NCC White Table" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="firstColumn" dxfId="22"/>
-      <tableStyleElement type="lastColumn" dxfId="21"/>
-      <tableStyleElement type="firstRowStripe" dxfId="20"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="totalRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
+      <tableStyleElement type="lastColumn" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="21"/>
     </tableStyle>
     <tableStyle name="PivotNCCDefaultBlue" table="0" count="14" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="totalRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="14"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="secondColumnSubheading" dxfId="10"/>
-      <tableStyleElement type="thirdColumnSubheading" dxfId="9"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="8"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="7"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="6"/>
-      <tableStyleElement type="pageFieldValues" dxfId="5"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
+      <tableStyleElement type="secondColumnSubheading" dxfId="12"/>
+      <tableStyleElement type="thirdColumnSubheading" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1459,38 +1477,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E22A2325-3E08-4CDD-B40F-7E0B52F68F7E}" name="Table2" displayName="Table2" ref="A1:D36" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D36" xr:uid="{12F0A6E3-9939-4F36-9F23-9E566736150C}"/>
-  <sortState ref="A2:D36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E22A2325-3E08-4CDD-B40F-7E0B52F68F7E}" name="Table2" displayName="Table2" ref="A1:C36" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:C36" xr:uid="{12F0A6E3-9939-4F36-9F23-9E566736150C}"/>
+  <sortState ref="A2:C36">
+    <sortCondition ref="C2:C36"/>
     <sortCondition ref="A2:A36"/>
-    <sortCondition ref="B2:B36"/>
-    <sortCondition ref="D2:D36"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="3">
     <tableColumn id="4" xr3:uid="{77D604CD-999B-4603-A942-A67E11167BDA}" name="cat1"/>
-    <tableColumn id="6" xr3:uid="{C9A15DA4-CE7C-470A-A631-C13EF92E1284}" name="cat2"/>
     <tableColumn id="1" xr3:uid="{E00B5BA3-1660-4ACA-BD4D-87910B07DA6B}" name="Condition description"/>
-    <tableColumn id="2" xr3:uid="{BD7E279D-637E-4828-970E-BB2161792735}" name="primary diagnosis" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BD7E279D-637E-4828-970E-BB2161792735}" name="primary diagnosis detail" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="NCC White Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6428CD34-B99A-449C-BD75-92CB38E0302C}" name="Table225" displayName="Table225" ref="A1:K14" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:K14" xr:uid="{34C5B988-CB0B-48F9-8C55-CD3937E4AD79}"/>
-  <sortState ref="A2:G14">
-    <sortCondition ref="A2:A34"/>
-    <sortCondition ref="B2:B34"/>
-    <sortCondition ref="E2:E34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6428CD34-B99A-449C-BD75-92CB38E0302C}" name="Table225" displayName="Table225" ref="A1:J14" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:J14" xr:uid="{34C5B988-CB0B-48F9-8C55-CD3937E4AD79}"/>
+  <sortState ref="A2:J14">
+    <sortCondition ref="D2:D14"/>
+    <sortCondition ref="A2:A14"/>
+    <sortCondition ref="B2:B14"/>
   </sortState>
-  <tableColumns count="11">
-    <tableColumn id="4" xr3:uid="{24E9D885-27DA-485D-8ED9-0816ADED6CA2}" name="cat1"/>
-    <tableColumn id="6" xr3:uid="{13906DF1-45F9-4BB4-8432-0BDA25CBF305}" name="cat2"/>
+  <tableColumns count="10">
+    <tableColumn id="4" xr3:uid="{24E9D885-27DA-485D-8ED9-0816ADED6CA2}" name="cat1" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{13906DF1-45F9-4BB4-8432-0BDA25CBF305}" name="cat2" dataDxfId="1"/>
     <tableColumn id="1" xr3:uid="{9E861F73-7DDD-43B0-A504-64B3944D7CC4}" name="Condition description"/>
-    <tableColumn id="3" xr3:uid="{CC12F7DB-1403-41D7-BAE0-1E3344E57E4E}" name="age"/>
-    <tableColumn id="2" xr3:uid="{8BB264FC-63E0-4EAE-B382-6737889E0292}" name="primary diagnosis" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{1333528A-B35E-42D7-8D0D-BDA8148950B2}" name="secondary diagnoses" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8BB264FC-63E0-4EAE-B382-6737889E0292}" name="primary diagnosis" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1333528A-B35E-42D7-8D0D-BDA8148950B2}" name="secondary diagnoses" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{552BB330-A267-471F-AA74-BB143F22FC48}" name="procedures"/>
     <tableColumn id="10" xr3:uid="{37FDC531-A372-42C5-9DCA-F71DE66EAF52}" name="prim_diag_regexp"/>
     <tableColumn id="9" xr3:uid="{152684CE-BB8F-4D6A-B72F-F7F80E6C2980}" name="sec_diag_include_regexp"/>
@@ -1843,7 +1858,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f ca="1">TODAY()</f>
-        <v>43539</v>
+        <v>43543</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1944,522 +1959,413 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F526BF-D9A6-4A08-87CA-ADC99D6ACA94}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>97</v>
-      </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>90</v>
       </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>90</v>
       </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>90</v>
       </c>
-      <c r="C20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>90</v>
       </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>76</v>
       </c>
-      <c r="C29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2475,316 +2381,271 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645F42B4-D193-4C4D-8A1D-36E8399E4942}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>14</v>
+    <row r="1" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="F8" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" t="s">
         <v>110</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="J11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
         <v>118</v>
-      </c>
-      <c r="K5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" t="s">
-        <v>119</v>
-      </c>
-      <c r="K6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[project] Some cosmetic changes to .xlsx - Excel fuss not content change.
</commit_message>
<xml_diff>
--- a/data-raw/acs_lus.xlsx
+++ b/data-raw/acs_lus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{66279789-0A59-4E66-A20F-90D0D8BB51AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{71F7ACE4-7D5B-4D9B-BB26-8726D026A513}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="12570" windowHeight="7770" tabRatio="421" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,6 +623,20 @@
   </cellStyles>
   <dxfs count="39">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -635,20 +649,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1501,11 +1501,11 @@
     <sortCondition ref="B2:B14"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="4" xr3:uid="{24E9D885-27DA-485D-8ED9-0816ADED6CA2}" name="cat1" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{13906DF1-45F9-4BB4-8432-0BDA25CBF305}" name="cat2" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{24E9D885-27DA-485D-8ED9-0816ADED6CA2}" name="cat1" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{13906DF1-45F9-4BB4-8432-0BDA25CBF305}" name="cat2" dataDxfId="2"/>
     <tableColumn id="1" xr3:uid="{9E861F73-7DDD-43B0-A504-64B3944D7CC4}" name="Condition description"/>
-    <tableColumn id="2" xr3:uid="{8BB264FC-63E0-4EAE-B382-6737889E0292}" name="primary diagnosis" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{1333528A-B35E-42D7-8D0D-BDA8148950B2}" name="secondary diagnoses" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{8BB264FC-63E0-4EAE-B382-6737889E0292}" name="primary diagnosis" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1333528A-B35E-42D7-8D0D-BDA8148950B2}" name="secondary diagnoses" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{552BB330-A267-471F-AA74-BB143F22FC48}" name="procedures"/>
     <tableColumn id="10" xr3:uid="{37FDC531-A372-42C5-9DCA-F71DE66EAF52}" name="prim_diag_regexp"/>
     <tableColumn id="9" xr3:uid="{152684CE-BB8F-4D6A-B72F-F7F80E6C2980}" name="sec_diag_include_regexp"/>
@@ -1858,7 +1858,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f ca="1">TODAY()</f>
-        <v>43543</v>
+        <v>43547</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2383,7 +2383,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>